<commit_message>
remove empty Excel sheets from neut data
Some Excel sheets had blank sheets without
neutralization data that were causing problems.
</commit_message>
<xml_diff>
--- a/data/neut_assays/plate_reader_data/571v1_NeutralizationAssay.xlsx
+++ b/data/neut_assays/plate_reader_data/571v1_NeutralizationAssay.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/computational_notebooks/jbloom/2019/map_flu_serum_Perth2009_H3_HA/data/neut_assays/plate_reader_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F976AB9B-AB18-D340-A65B-98F8772EF0B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="180" windowWidth="27800" windowHeight="12580"/>
+    <workbookView xWindow="2300" yWindow="460" windowWidth="27800" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Lee, Juhye M</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,19 +413,22 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6"/>
-    <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7"/>
-    <cellStyle name="Tecan.At.Excel.Error" xfId="1"/>
-    <cellStyle name="Tecan.At.Excel.GFactorAndMeasurementBlank" xfId="5"/>
-    <cellStyle name="Tecan.At.Excel.GFactorBlank" xfId="3"/>
-    <cellStyle name="Tecan.At.Excel.GFactorReference" xfId="4"/>
-    <cellStyle name="Tecan.At.Excel.MeasurementBlank" xfId="2"/>
+    <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Tecan.At.Excel.Error" xfId="1" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorAndMeasurementBlank" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorBlank" xfId="3" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorReference" xfId="4" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Tecan.At.Excel.MeasurementBlank" xfId="2" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -712,16 +720,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -729,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -737,7 +745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -745,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -753,7 +761,7 @@
         <v>43375</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -761,7 +769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -769,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -777,7 +785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -785,17 +793,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -803,12 +811,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -819,7 +827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -830,7 +838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -841,7 +849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -852,7 +860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -863,7 +871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -874,7 +882,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -885,7 +893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -896,7 +904,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -907,7 +915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -918,7 +926,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -926,12 +934,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -972,12 +980,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1018,7 +1026,7 @@
         <v>10769</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1059,7 +1067,7 @@
         <v>34207</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1100,7 +1108,7 @@
         <v>35333</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1141,7 +1149,7 @@
         <v>31573</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>33165</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -1223,12 +1231,12 @@
         <v>33182</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1246,21 +1254,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>